<commit_message>
Add checklist xml to 4COM01_RANESeqGEO.xlsx
</commit_message>
<xml_diff>
--- a/templates/4COM01_RNASeqGEO/4COM01_RNASeqGEO.xlsx
+++ b/templates/4COM01_RNASeqGEO/4COM01_RNASeqGEO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/Transcriptomics_GEO/03_SWATEtemplate_v1.0.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Freym\source\repos\SWATE_templates\templates\4COM01_RNASeqGEO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1650C248-8CB4-3547-9081-6F0821AF5159}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E2A03D-D59D-420D-880D-BBBC21DB5B97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4720" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-28920" yWindow="-6555" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM01_RNASeqGEO" sheetId="5" r:id="rId1"/>
@@ -607,7 +607,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="710" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -627,47 +627,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBB40E6-F06B-AE48-B869-B32AACDBDD09}">
   <dimension ref="A1:DE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="62.3125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="68.5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.3125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="75.1640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="75.1875" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="72.8125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="79" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="64.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="64.6875" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="71" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="42.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="71.6640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="77.83203125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42.8125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="71.6875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="77.8125" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="46.3125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="75" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="81.33203125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="67.1640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="73.33203125" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="81.3125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="38.3125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="67.1875" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="73.3125" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="64.1640625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="64.1875" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="70.5" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="65.33203125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="65.3125" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="71.5" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="39" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="67.83203125" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="67.8125" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="74" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:109" x14ac:dyDescent="0.5">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -701,7 +701,7 @@
       <c r="AE1" s="4"/>
       <c r="AF1" s="2"/>
     </row>
-    <row r="2" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:109" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -799,7 +799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:109" x14ac:dyDescent="0.5">
       <c r="C3" s="3"/>
       <c r="F3" s="3"/>
       <c r="I3" s="3"/>
@@ -819,4 +819,31 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<customXml>
+  <SwateTable Table="annotationTable3" Worksheet="4COM01_RNASeqGEO">
+    <TableValidation DateTime="2021-03-11 15:14" SwateVersion="0.4.4" TableName="annotationTable3" Userlist="" WorksheetName="4COM01_RNASeqGEO">
+      <ColumnValidation ColumnAdress="0" ColumnHeader="Source Name" Importance="5" Unit="None" ValidationFormat="Text"/>
+      <ColumnValidation ColumnAdress="1" ColumnHeader="Sample Name" Importance="5" Unit="None" ValidationFormat="Text"/>
+      <ColumnValidation ColumnAdress="2" ColumnHeader="Parameter [Data filtering software]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="5" ColumnHeader="Parameter [Data filtering software version]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="8" ColumnHeader="Parameter [Data filtering Software Parameters]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="11" ColumnHeader="Parameter [Read Alignment Software]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="14" ColumnHeader="Parameter [Read Alignment Software Version]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="17" ColumnHeader="Parameter [Read Alignment Software Parameters]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="20" ColumnHeader="Parameter [Genome reference sequence]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="23" ColumnHeader="Parameter [Processed data file name]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="26" ColumnHeader="Parameter [Processed data file format]" Importance="None" Unit="None" ValidationFormat="None"/>
+      <ColumnValidation ColumnAdress="29" ColumnHeader="Parameter [Processed data file checksum]" Importance="None" Unit="None" ValidationFormat="None"/>
+    </TableValidation>
+  </SwateTable>
+</customXml>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D14FF22E-B337-4D83-88E8-158F9B8E1582}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adapted according to Angela's review
</commit_message>
<xml_diff>
--- a/templates/4COM01_RNASeqGEO/4COM01_RNASeqGEO.xlsx
+++ b/templates/4COM01_RNASeqGEO/4COM01_RNASeqGEO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Freym\source\repos\SWATE_templates\templates\4COM01_RNASeqGEO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Google Drive/CEPLAS/DataManagementPlans/SWATE_templates/templates/4COM01_RNASeqGEO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E2A03D-D59D-420D-880D-BBBC21DB5B97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D19E4C-CDA9-D34D-A295-6678CF914057}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6555" windowWidth="29040" windowHeight="15840" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
+    <workbookView xWindow="-4760" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{BA2B9B0E-8C9E-F34F-95FF-EF6336B60454}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM01_RNASeqGEO" sheetId="5" r:id="rId1"/>
@@ -24,8 +24,81 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Dominik Brilhaus</author>
+  </authors>
+  <commentList>
+    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{140CBE1F-7B48-134E-9B41-9BC85F1D4E84}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dominik Brilhaus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">cv: controlled vocabulary
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">m: mandatory 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">o: optional (can be mapped)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>n: not required (cannot be mapped)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
   <si>
     <t>Source Name</t>
   </si>
@@ -121,13 +194,191 @@
   </si>
   <si>
     <t>Term Accession Number [Processed data file checksum] (#h; #tNFDI4PSO:0000029)</t>
+  </si>
+  <si>
+    <t>SWATE annotation table</t>
+  </si>
+  <si>
+    <t>Content examples</t>
+  </si>
+  <si>
+    <t>Semantic Modelling</t>
+  </si>
+  <si>
+    <t>Term Name</t>
+  </si>
+  <si>
+    <t>Term Accession Number (TAN)</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>is_a</t>
+  </si>
+  <si>
+    <t>is_a URI</t>
+  </si>
+  <si>
+    <t>Content type (Validation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment: </t>
+  </si>
+  <si>
+    <t>ER Pipeline: GEO - RNASeq - Plants</t>
+  </si>
+  <si>
+    <t>ER target term</t>
+  </si>
+  <si>
+    <t>ER requirement (cv/m/o/n)</t>
+  </si>
+  <si>
+    <t>Importance (0-5)</t>
+  </si>
+  <si>
+    <t>Justification</t>
+  </si>
+  <si>
+    <t>Additional information</t>
+  </si>
+  <si>
+    <t>User instruction</t>
+  </si>
+  <si>
+    <t>Review comments</t>
+  </si>
+  <si>
+    <t>Trimmomatic</t>
+  </si>
+  <si>
+    <t>GENEPIO_0002096: read adapter trimming software</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0002096</t>
+  </si>
+  <si>
+    <t>Kallisto</t>
+  </si>
+  <si>
+    <t>HiSat2</t>
+  </si>
+  <si>
+    <t>STAR</t>
+  </si>
+  <si>
+    <t>BWA</t>
+  </si>
+  <si>
+    <t>0.45.1</t>
+  </si>
+  <si>
+    <t>kallisto quant -b 50 -t 10</t>
+  </si>
+  <si>
+    <t>.xlsx</t>
+  </si>
+  <si>
+    <t>.txt</t>
+  </si>
+  <si>
+    <t>.csv</t>
+  </si>
+  <si>
+    <t>Data filtering Software</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000023</t>
+  </si>
+  <si>
+    <t>Data filtering Software Version</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000024</t>
+  </si>
+  <si>
+    <t>Data filtering Software Parameters</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000025</t>
+  </si>
+  <si>
+    <t>Read Alignment Software</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000002</t>
+  </si>
+  <si>
+    <t>Read Alignment Software Version</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000003</t>
+  </si>
+  <si>
+    <t>Read Alignment Software Parameters</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000004</t>
+  </si>
+  <si>
+    <t>Genome reference sequence</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000026</t>
+  </si>
+  <si>
+    <t>Processed data file format</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000027</t>
+  </si>
+  <si>
+    <t>Processed data file name</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000028</t>
+  </si>
+  <si>
+    <t>Processed data file checksum</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000029</t>
+  </si>
+  <si>
+    <t>MD5 checksum</t>
+  </si>
+  <si>
+    <t>data_processing_pipeline.data_processing_step</t>
+  </si>
+  <si>
+    <t>data_processing_pipeline.genome_build</t>
+  </si>
+  <si>
+    <t>processed_data_files.file_name</t>
+  </si>
+  <si>
+    <t>processed_data_files.file_type</t>
+  </si>
+  <si>
+    <t>processed_data_files.file_checksum</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Also maps to:
+data_processing_pipeline.processed_data_files_format_and_content</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,8 +394,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,8 +456,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4FB3D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF377D98"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -195,20 +530,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -220,10 +547,75 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{C330E3B2-2BF7-184E-8C2F-47A51BE085E3}"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -270,8 +662,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B1E8DF05-C9A4-774C-927F-FE22EC52758A}" name="annotationTable3" displayName="annotationTable3" ref="A2:AF3" totalsRowShown="0">
-  <autoFilter ref="A2:AF3" xr:uid="{856B7222-837D-994E-B57E-2C90FB73CB67}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B1E8DF05-C9A4-774C-927F-FE22EC52758A}" name="annotationTable3" displayName="annotationTable3" ref="C2:AH3" totalsRowShown="0">
+  <autoFilter ref="C2:AH3" xr:uid="{856B7222-837D-994E-B57E-2C90FB73CB67}"/>
   <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{FFCB64B6-F7E5-3141-8AC8-90DEF404CB27}" name="Source Name"/>
     <tableColumn id="2" xr3:uid="{83E02E49-7422-0646-B55C-39A1A7410443}" name="Sample Name"/>
@@ -607,7 +999,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="710" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -624,53 +1016,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBB40E6-F06B-AE48-B869-B32AACDBDD09}">
-  <dimension ref="A1:DE3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBB40E6-F06B-AE48-B869-B32AACDBDD09}">
+  <dimension ref="A1:AH29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.3125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="68.5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="40.3125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="75.1875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.8125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="79" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="64.6875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="71" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="42.8125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="71.6875" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="77.8125" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="46.3125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="75" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="81.3125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="38.3125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="67.1875" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="73.3125" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="64.1875" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="70.5" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="65.3125" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="71.5" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="39" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="67.8125" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="74" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="29" customWidth="1"/>
+    <col min="6" max="6" width="62.33203125" style="29" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="68.5" style="29" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="33.83203125" style="29" customWidth="1"/>
+    <col min="9" max="9" width="69" style="29" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="75.1640625" style="29" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="44" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="72.83203125" style="29" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="79" style="29" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="41.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="64.6640625" style="29" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="71" style="29" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="42.83203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="71.6640625" style="29" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="77.83203125" style="29" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="46.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="75" style="29" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="81.33203125" style="29" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="38.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="67.1640625" style="29" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="73.33203125" style="29" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="35.5" style="29" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="64.1640625" style="29" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="70.5" style="29" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="36.5" style="29" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="65.33203125" style="29" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="71.5" style="29" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="39" style="29" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="67.83203125" style="29" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="74" style="29" hidden="1" customWidth="1"/>
+    <col min="35" max="16384" width="11" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" x14ac:dyDescent="0.5">
-      <c r="A1" s="1"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+    <row r="1" spans="1:34" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -699,124 +1099,1269 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
-      <c r="AF1" s="2"/>
-    </row>
-    <row r="2" spans="1:109" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="2"/>
+    </row>
+    <row r="2" spans="1:34" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>18</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>19</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>20</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>21</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>22</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.5">
-      <c r="C3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="DE3" s="5"/>
+    <row r="3" spans="1:34" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3" s="3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" s="3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3" s="3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3" s="3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3" s="3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3" s="3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="23"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="23"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
+      <c r="AA6" s="23"/>
+      <c r="AB6" s="23"/>
+      <c r="AC6" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD6" s="23"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="23"/>
+      <c r="AG6" s="23"/>
+      <c r="AH6" s="23"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="23"/>
+      <c r="AF7" s="23"/>
+      <c r="AG7" s="23"/>
+      <c r="AH7" s="23"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23"/>
+      <c r="AE8" s="23"/>
+      <c r="AF8" s="23"/>
+      <c r="AG8" s="23"/>
+      <c r="AH8" s="23"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="23"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
+      <c r="Z9" s="23"/>
+      <c r="AA9" s="23"/>
+      <c r="AB9" s="23"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="23"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
+      <c r="AH9" s="23"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="22"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="24"/>
+      <c r="Z11" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA11" s="24"/>
+      <c r="AB11" s="24"/>
+      <c r="AC11" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD11" s="24"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG11" s="24"/>
+      <c r="AH11" s="24"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="25"/>
+      <c r="AC12" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD12" s="25"/>
+      <c r="AE12" s="25"/>
+      <c r="AF12" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG12" s="25"/>
+      <c r="AH12" s="25"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="20"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="20"/>
+      <c r="AG13" s="20"/>
+      <c r="AH13" s="20"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="20"/>
+      <c r="AF14" s="20"/>
+      <c r="AG14" s="20"/>
+      <c r="AH14" s="20"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="W15" s="26"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
+      <c r="AA15" s="26"/>
+      <c r="AB15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="26"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="26"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27"/>
+      <c r="AA16" s="27"/>
+      <c r="AB16" s="27"/>
+      <c r="AC16" s="27"/>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="27"/>
+      <c r="AF16" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG16" s="27"/>
+      <c r="AH16" s="27"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="20"/>
+      <c r="AC17" s="20"/>
+      <c r="AD17" s="20"/>
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="20"/>
+      <c r="AH17" s="20"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="20"/>
+      <c r="AC18" s="20"/>
+      <c r="AD18" s="20"/>
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="20"/>
+      <c r="S19" s="20"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="20"/>
+      <c r="AB19" s="20"/>
+      <c r="AC19" s="20"/>
+      <c r="AD19" s="20"/>
+      <c r="AE19" s="20"/>
+      <c r="AF19" s="20"/>
+      <c r="AG19" s="20"/>
+      <c r="AH19" s="20"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="28"/>
+      <c r="AC20" s="28"/>
+      <c r="AD20" s="28"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="28"/>
+      <c r="AH20" s="28"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="28"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="28"/>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="28"/>
+      <c r="AD21" s="28"/>
+      <c r="AE21" s="28"/>
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="28"/>
+      <c r="AH21" s="28"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="W22" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z22" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC22" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF22" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG22" s="20"/>
+      <c r="AH22" s="20"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD23" s="20"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="20"/>
+      <c r="AG23" s="20"/>
+      <c r="AH23" s="20"/>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="20"/>
+      <c r="AE24" s="20"/>
+      <c r="AF24" s="20"/>
+      <c r="AG24" s="20"/>
+      <c r="AH24" s="20"/>
+    </row>
+    <row r="25" spans="1:34" s="33" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25" s="21"/>
+      <c r="AA25" s="21"/>
+      <c r="AB25" s="21"/>
+      <c r="AC25" s="21"/>
+      <c r="AD25" s="21"/>
+      <c r="AE25" s="21"/>
+      <c r="AF25" s="21"/>
+      <c r="AG25" s="21"/>
+      <c r="AH25" s="21"/>
+    </row>
+    <row r="26" spans="1:34" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA26" s="30"/>
+      <c r="AB26" s="30"/>
+      <c r="AC26" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD26" s="21"/>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="21"/>
+      <c r="AG26" s="21"/>
+      <c r="AH26" s="21"/>
+    </row>
+    <row r="27" spans="1:34" s="33" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="21"/>
+      <c r="Z27" s="21"/>
+      <c r="AA27" s="21"/>
+      <c r="AB27" s="21"/>
+      <c r="AC27" s="21"/>
+      <c r="AD27" s="21"/>
+      <c r="AE27" s="21"/>
+      <c r="AF27" s="21"/>
+      <c r="AG27" s="21"/>
+      <c r="AH27" s="21"/>
+    </row>
+    <row r="28" spans="1:34" s="33" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
+      <c r="X28" s="35"/>
+      <c r="Y28" s="35"/>
+      <c r="Z28" s="35"/>
+      <c r="AA28" s="35"/>
+      <c r="AB28" s="35"/>
+      <c r="AC28" s="35"/>
+      <c r="AD28" s="35"/>
+      <c r="AE28" s="35"/>
+      <c r="AF28" s="35"/>
+      <c r="AG28" s="35"/>
+      <c r="AH28" s="35"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
+      <c r="R29" s="22"/>
+      <c r="S29" s="22"/>
+      <c r="T29" s="22"/>
+      <c r="U29" s="22"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="22"/>
+      <c r="Y29" s="22"/>
+      <c r="Z29" s="22"/>
+      <c r="AA29" s="22"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="22"/>
+      <c r="AD29" s="22"/>
+      <c r="AE29" s="22"/>
+      <c r="AF29" s="22"/>
+      <c r="AG29" s="22"/>
+      <c r="AH29" s="22"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E15" r:id="rId1" xr:uid="{637B5E25-8D6F-4E4B-9B44-BCD0C6366524}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>